<commit_message>
Extended rows to fit more players
</commit_message>
<xml_diff>
--- a/color.xlsx
+++ b/color.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\stats tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36493BA1-1F87-455A-84F6-B064546AA689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580FD31B-17FD-4D02-9252-B2AF16573C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{197E854B-D497-46FC-AC16-9B33D52D7071}"/>
   </bookViews>
@@ -87,13 +87,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor rgb="FF5B9BD5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,6 +201,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF5B9BD5"/>
       <color rgb="FFDE2241"/>
     </mruColors>
   </colors>
@@ -512,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72C6D35-6CB8-4F1B-A36B-80757C15C00B}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,280 +548,280 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -834,10 +835,10 @@
       <c r="O37" s="1"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -851,10 +852,10 @@
       <c r="O38" s="1"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -867,9 +868,411 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="6"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="6"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="6"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="6"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="6"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B36">
-    <cfRule type="colorScale" priority="21">
+  <conditionalFormatting sqref="B2:B106">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -879,7 +1282,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -888,18 +1291,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C31">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFC00000"/>
-        <color theme="9"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C2:C36">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -909,7 +1302,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -917,9 +1310,17 @@
         <color theme="9"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D36">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -927,7 +1328,7 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -937,19 +1338,99 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N37:N68">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="INVOIT">
+    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="INVOIT">
       <formula>NOT(ISERROR(SEARCH("INVOIT",N37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="INACTIVITATE">
+    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="INACTIVITATE">
       <formula>NOT(ISERROR(SEARCH("INACTIVITATE",N37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O37:O63">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="INVOIT">
+    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="INVOIT">
       <formula>NOT(ISERROR(SEARCH("INVOIT",O37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="INACTIVITATE">
+    <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="INACTIVITATE">
       <formula>NOT(ISERROR(SEARCH("INACTIVITATE",O37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C71">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C72:C106">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:D71">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D72:D106">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="9"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed excel formating bug
</commit_message>
<xml_diff>
--- a/color.xlsx
+++ b/color.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\stats tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580FD31B-17FD-4D02-9252-B2AF16573C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48179603-F753-4DEB-BCCE-DA7947A39113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{197E854B-D497-46FC-AC16-9B33D52D7071}"/>
   </bookViews>
@@ -138,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,13 +155,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72C6D35-6CB8-4F1B-A36B-80757C15C00B}">
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,279 +543,279 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -836,9 +830,9 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -853,9 +847,9 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -870,405 +864,405 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="7"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="7"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="7"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-      <c r="D87" s="7"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
-      <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="7"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="7"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="7"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="6"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
+      <c r="A102" s="5"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="6"/>
-      <c r="B103" s="8"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
+      <c r="A103" s="5"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="6"/>
-      <c r="B104" s="8"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
+      <c r="A104" s="5"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="6"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
+      <c r="A105" s="5"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
+      <c r="A106" s="5"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B106">
@@ -1319,40 +1313,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D36">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFC00000"/>
-        <color theme="9"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N37:N68">
-    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="INVOIT">
-      <formula>NOT(ISERROR(SEARCH("INVOIT",N37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="INACTIVITATE">
-      <formula>NOT(ISERROR(SEARCH("INACTIVITATE",N37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O37:O63">
-    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="INVOIT">
-      <formula>NOT(ISERROR(SEARCH("INVOIT",O37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="INACTIVITATE">
-      <formula>NOT(ISERROR(SEARCH("INACTIVITATE",O37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C37:C71">
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -1393,6 +1353,24 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D36">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D37:D71">
     <cfRule type="colorScale" priority="3">
       <colorScale>
@@ -1433,6 +1411,22 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N37:N68">
+    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="INVOIT">
+      <formula>NOT(ISERROR(SEARCH("INVOIT",N37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="INACTIVITATE">
+      <formula>NOT(ISERROR(SEARCH("INACTIVITATE",N37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O37:O63">
+    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="INVOIT">
+      <formula>NOT(ISERROR(SEARCH("INVOIT",O37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="INACTIVITATE">
+      <formula>NOT(ISERROR(SEARCH("INACTIVITATE",O37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>